<commit_message>
some flex but needs Q fixing
</commit_message>
<xml_diff>
--- a/circuits/net3.xlsx
+++ b/circuits/net3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshil\Desktop\4thyear\python\final code\circuits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E457D9-61B1-4AA1-A88D-79BF4F498A27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9A10B6-3B70-41C2-9C73-826C1BEF31F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="914" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1307,9 +1307,6 @@
     <t>PV 5r</t>
   </si>
   <si>
-    <t>PV 6r</t>
-  </si>
-  <si>
     <t>CHP diesel 1r</t>
   </si>
   <si>
@@ -1350,6 +1347,9 @@
   </si>
   <si>
     <t>CHP diesel 7rc</t>
+  </si>
+  <si>
+    <t>CHP diesel 2r</t>
   </si>
 </sst>
 </file>
@@ -11971,7 +11971,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12185,7 +12185,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>4.0000000000000001E-3</v>
+        <v>0.5</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -12194,7 +12194,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -12205,7 +12205,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>414</v>
+        <v>427</v>
       </c>
       <c r="C8">
         <v>18</v>
@@ -12237,7 +12237,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C9">
         <v>24</v>
@@ -12269,7 +12269,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C10">
         <v>59</v>
@@ -12301,7 +12301,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C11">
         <v>62</v>
@@ -12333,7 +12333,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C12">
         <v>61</v>
@@ -12365,7 +12365,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C13">
         <v>57</v>
@@ -12397,7 +12397,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C14">
         <v>35</v>
@@ -12429,7 +12429,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C15">
         <v>33</v>
@@ -12461,7 +12461,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C16">
         <v>63</v>
@@ -12493,7 +12493,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C17">
         <v>52</v>
@@ -12637,7 +12637,7 @@
   <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13964,8 +13964,8 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14962,7 +14962,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C22" t="s">
         <v>328</v>
@@ -16701,7 +16701,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C59" t="s">
         <v>326</v>
@@ -16748,7 +16748,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C60" t="s">
         <v>326</v>
@@ -16795,7 +16795,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C61" t="s">
         <v>329</v>

</xml_diff>

<commit_message>
Final Code Upload and cleanup
</commit_message>
<xml_diff>
--- a/circuits/net3.xlsx
+++ b/circuits/net3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshil\Desktop\4thyear\python\final code\circuits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA07A253-E4E0-49D0-8122-A385F806BC1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BFF349-05D0-45A5-A2EF-ACA1BBBD5528}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="914" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="420">
   <si>
     <t>element</t>
   </si>
@@ -1148,7 +1148,184 @@
     <t>Battery 2</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Line main</t>
+  </si>
+  <si>
+    <t>Line R0-R1</t>
+  </si>
+  <si>
+    <t>Line R1-R2</t>
+  </si>
+  <si>
+    <t>Line R2-R3</t>
+  </si>
+  <si>
+    <t>Line R3-R4</t>
+  </si>
+  <si>
+    <t>Line R4-R5</t>
+  </si>
+  <si>
+    <t>Line R5-R6</t>
+  </si>
+  <si>
+    <t>Line R6-R7</t>
+  </si>
+  <si>
+    <t>Line R7-R8</t>
+  </si>
+  <si>
+    <t>Line R8-R9</t>
+  </si>
+  <si>
+    <t>Line R9-R10</t>
+  </si>
+  <si>
+    <t>Line R3-R11</t>
+  </si>
+  <si>
+    <t>Line R4-R12</t>
+  </si>
+  <si>
+    <t>Line R12-R13</t>
+  </si>
+  <si>
+    <t>Line R13-R14</t>
+  </si>
+  <si>
+    <t>Line R14-R15</t>
+  </si>
+  <si>
+    <t>Line R6-R16</t>
+  </si>
+  <si>
+    <t>Line R9-R17</t>
+  </si>
+  <si>
+    <t>Line R10-R18</t>
+  </si>
+  <si>
+    <t>Line I0-I1</t>
+  </si>
+  <si>
+    <t>Line I1-I2</t>
+  </si>
+  <si>
+    <t>Line I1-I3</t>
+  </si>
+  <si>
+    <t>Line I2-I3</t>
+  </si>
+  <si>
+    <t>Line C0-C1</t>
+  </si>
+  <si>
+    <t>Line C1-C2</t>
+  </si>
+  <si>
+    <t>Line C2-C3</t>
+  </si>
+  <si>
+    <t>Line C3-C4</t>
+  </si>
+  <si>
+    <t>Line C4-C5</t>
+  </si>
+  <si>
+    <t>Line C5-C6</t>
+  </si>
+  <si>
+    <t>Line C6-C7</t>
+  </si>
+  <si>
+    <t>Line C7-C8</t>
+  </si>
+  <si>
+    <t>Line C8-C9</t>
+  </si>
+  <si>
+    <t>Line C3-C10</t>
+  </si>
+  <si>
+    <t>Line C10-C11</t>
+  </si>
+  <si>
+    <t>Line C11-C12</t>
+  </si>
+  <si>
+    <t>Line C11-C13</t>
+  </si>
+  <si>
+    <t>Line C10-C14</t>
+  </si>
+  <si>
+    <t>Line C5-C15</t>
+  </si>
+  <si>
+    <t>Line C15-C16</t>
+  </si>
+  <si>
+    <t>Line C15-C17</t>
+  </si>
+  <si>
+    <t>Line C16-C18</t>
+  </si>
+  <si>
+    <t>Line C8-C19</t>
+  </si>
+  <si>
+    <t>Line C9-C20</t>
+  </si>
+  <si>
+    <t>Line RC0-RC1</t>
+  </si>
+  <si>
+    <t>Line RC1-RC2</t>
+  </si>
+  <si>
+    <t>Line RC2-RC3</t>
+  </si>
+  <si>
+    <t>Line RC3-RC4</t>
+  </si>
+  <si>
+    <t>Line RC4-RC5</t>
+  </si>
+  <si>
+    <t>Line RC5-RC6</t>
+  </si>
+  <si>
+    <t>Line RC2-RC8</t>
+  </si>
+  <si>
+    <t>Line RC8-RC9</t>
+  </si>
+  <si>
+    <t>Line RC9-RC10</t>
+  </si>
+  <si>
+    <t>Line RC10-RC11</t>
+  </si>
+  <si>
+    <t>Line RC11-RC12</t>
+  </si>
+  <si>
+    <t>Line RC12-RC13</t>
+  </si>
+  <si>
+    <t>Line RC13-RC14</t>
+  </si>
+  <si>
+    <t>Line RC14-RC15</t>
+  </si>
+  <si>
+    <t>Line RC12-RC16</t>
+  </si>
+  <si>
+    <t>Line RC16-RC17</t>
+  </si>
+  <si>
+    <t>Line RC17-RC18</t>
   </si>
 </sst>
 </file>
@@ -1178,12 +1355,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -1224,7 +1413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1239,6 +1428,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12110,7 +12301,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
@@ -12235,11 +12426,6 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I25" t="s">
-        <v>360</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -13579,13 +13765,16 @@
   <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D1:E61"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
       <c r="C1" s="1" t="s">
         <v>82</v>
       </c>
@@ -13630,6 +13819,9 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>360</v>
+      </c>
       <c r="C2" t="s">
         <v>272</v>
       </c>
@@ -13673,6 +13865,9 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>361</v>
       </c>
       <c r="C3" t="s">
         <v>269</v>
@@ -13718,6 +13913,9 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="B4" s="6" t="s">
+        <v>362</v>
+      </c>
       <c r="C4" t="s">
         <v>269</v>
       </c>
@@ -13762,6 +13960,9 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
+      <c r="B5" s="6" t="s">
+        <v>363</v>
+      </c>
       <c r="C5" t="s">
         <v>269</v>
       </c>
@@ -13806,6 +14007,9 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="B6" s="7" t="s">
+        <v>364</v>
+      </c>
       <c r="C6" t="s">
         <v>269</v>
       </c>
@@ -13850,6 +14054,9 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="B7" s="7" t="s">
+        <v>365</v>
+      </c>
       <c r="C7" t="s">
         <v>269</v>
       </c>
@@ -13894,6 +14101,9 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
+      <c r="B8" s="7" t="s">
+        <v>366</v>
+      </c>
       <c r="C8" t="s">
         <v>269</v>
       </c>
@@ -13938,6 +14148,9 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>367</v>
+      </c>
       <c r="C9" t="s">
         <v>269</v>
       </c>
@@ -13982,6 +14195,9 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>368</v>
+      </c>
       <c r="C10" t="s">
         <v>269</v>
       </c>
@@ -14026,6 +14242,9 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>369</v>
+      </c>
       <c r="C11" t="s">
         <v>269</v>
       </c>
@@ -14070,6 +14289,9 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>370</v>
+      </c>
       <c r="C12" t="s">
         <v>269</v>
       </c>
@@ -14114,6 +14336,9 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>371</v>
+      </c>
       <c r="C13" t="s">
         <v>270</v>
       </c>
@@ -14158,6 +14383,9 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>372</v>
+      </c>
       <c r="C14" t="s">
         <v>270</v>
       </c>
@@ -14202,6 +14430,9 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>373</v>
+      </c>
       <c r="C15" t="s">
         <v>270</v>
       </c>
@@ -14246,6 +14477,9 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>374</v>
+      </c>
       <c r="C16" t="s">
         <v>270</v>
       </c>
@@ -14290,6 +14524,9 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>375</v>
+      </c>
       <c r="C17" t="s">
         <v>270</v>
       </c>
@@ -14334,6 +14571,9 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>376</v>
+      </c>
       <c r="C18" t="s">
         <v>270</v>
       </c>
@@ -14378,6 +14618,9 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
+      <c r="B19" t="s">
+        <v>377</v>
+      </c>
       <c r="C19" t="s">
         <v>270</v>
       </c>
@@ -14422,6 +14665,9 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
+      <c r="B20" t="s">
+        <v>378</v>
+      </c>
       <c r="C20" t="s">
         <v>270</v>
       </c>
@@ -14466,6 +14712,9 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
+      <c r="B21" s="6" t="s">
+        <v>379</v>
+      </c>
       <c r="C21" t="s">
         <v>271</v>
       </c>
@@ -14510,6 +14759,9 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
+      <c r="B22" s="7" t="s">
+        <v>380</v>
+      </c>
       <c r="C22" t="s">
         <v>271</v>
       </c>
@@ -14554,6 +14806,9 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
+      <c r="B23" t="s">
+        <v>381</v>
+      </c>
       <c r="C23" t="s">
         <v>271</v>
       </c>
@@ -14598,6 +14853,9 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
+      <c r="B24" t="s">
+        <v>382</v>
+      </c>
       <c r="C24" t="s">
         <v>271</v>
       </c>
@@ -14642,6 +14900,9 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
+      <c r="B25" s="6" t="s">
+        <v>383</v>
+      </c>
       <c r="C25" t="s">
         <v>272</v>
       </c>
@@ -14686,6 +14947,9 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
+      <c r="B26" s="6" t="s">
+        <v>384</v>
+      </c>
       <c r="C26" t="s">
         <v>272</v>
       </c>
@@ -14730,6 +14994,9 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
+      <c r="B27" s="6" t="s">
+        <v>385</v>
+      </c>
       <c r="C27" t="s">
         <v>272</v>
       </c>
@@ -14774,6 +15041,9 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
+      <c r="B28" s="7" t="s">
+        <v>386</v>
+      </c>
       <c r="C28" t="s">
         <v>272</v>
       </c>
@@ -14818,6 +15088,9 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
+      <c r="B29" s="7" t="s">
+        <v>387</v>
+      </c>
       <c r="C29" t="s">
         <v>272</v>
       </c>
@@ -14862,6 +15135,9 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
+      <c r="B30" t="s">
+        <v>388</v>
+      </c>
       <c r="C30" t="s">
         <v>272</v>
       </c>
@@ -14906,6 +15182,9 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
+      <c r="B31" t="s">
+        <v>389</v>
+      </c>
       <c r="C31" t="s">
         <v>272</v>
       </c>
@@ -14950,6 +15229,9 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
+      <c r="B32" t="s">
+        <v>390</v>
+      </c>
       <c r="C32" t="s">
         <v>272</v>
       </c>
@@ -14994,6 +15276,9 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
+      <c r="B33" t="s">
+        <v>391</v>
+      </c>
       <c r="C33" t="s">
         <v>272</v>
       </c>
@@ -15038,6 +15323,9 @@
       <c r="A34" s="1">
         <v>32</v>
       </c>
+      <c r="B34" t="s">
+        <v>392</v>
+      </c>
       <c r="C34" t="s">
         <v>273</v>
       </c>
@@ -15082,6 +15370,9 @@
       <c r="A35" s="1">
         <v>33</v>
       </c>
+      <c r="B35" t="s">
+        <v>393</v>
+      </c>
       <c r="C35" t="s">
         <v>273</v>
       </c>
@@ -15126,6 +15417,9 @@
       <c r="A36" s="1">
         <v>34</v>
       </c>
+      <c r="B36" t="s">
+        <v>394</v>
+      </c>
       <c r="C36" t="s">
         <v>274</v>
       </c>
@@ -15170,6 +15464,9 @@
       <c r="A37" s="1">
         <v>35</v>
       </c>
+      <c r="B37" t="s">
+        <v>395</v>
+      </c>
       <c r="C37" t="s">
         <v>274</v>
       </c>
@@ -15214,6 +15511,9 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
+      <c r="B38" t="s">
+        <v>396</v>
+      </c>
       <c r="C38" t="s">
         <v>274</v>
       </c>
@@ -15258,6 +15558,9 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
+      <c r="B39" s="7" t="s">
+        <v>397</v>
+      </c>
       <c r="C39" t="s">
         <v>273</v>
       </c>
@@ -15302,6 +15605,9 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
+      <c r="B40" t="s">
+        <v>398</v>
+      </c>
       <c r="C40" t="s">
         <v>273</v>
       </c>
@@ -15346,6 +15652,9 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
+      <c r="B41" t="s">
+        <v>399</v>
+      </c>
       <c r="C41" t="s">
         <v>274</v>
       </c>
@@ -15390,6 +15699,9 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
+      <c r="B42" t="s">
+        <v>400</v>
+      </c>
       <c r="C42" t="s">
         <v>274</v>
       </c>
@@ -15434,6 +15746,9 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
+      <c r="B43" t="s">
+        <v>401</v>
+      </c>
       <c r="C43" t="s">
         <v>274</v>
       </c>
@@ -15478,6 +15793,9 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
+      <c r="B44" t="s">
+        <v>402</v>
+      </c>
       <c r="C44" t="s">
         <v>274</v>
       </c>
@@ -15522,6 +15840,9 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
+      <c r="B45" s="6" t="s">
+        <v>403</v>
+      </c>
       <c r="C45" t="s">
         <v>269</v>
       </c>
@@ -15566,6 +15887,9 @@
       <c r="A46" s="1">
         <v>44</v>
       </c>
+      <c r="B46" s="6" t="s">
+        <v>404</v>
+      </c>
       <c r="C46" t="s">
         <v>269</v>
       </c>
@@ -15610,6 +15934,9 @@
       <c r="A47" s="1">
         <v>45</v>
       </c>
+      <c r="B47" t="s">
+        <v>405</v>
+      </c>
       <c r="C47" t="s">
         <v>269</v>
       </c>
@@ -15654,6 +15981,9 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
+      <c r="B48" t="s">
+        <v>406</v>
+      </c>
       <c r="C48" t="s">
         <v>269</v>
       </c>
@@ -15698,6 +16028,9 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
+      <c r="B49" t="s">
+        <v>407</v>
+      </c>
       <c r="C49" t="s">
         <v>269</v>
       </c>
@@ -15742,6 +16075,9 @@
       <c r="A50" s="1">
         <v>48</v>
       </c>
+      <c r="B50" t="s">
+        <v>408</v>
+      </c>
       <c r="C50" t="s">
         <v>269</v>
       </c>
@@ -15786,6 +16122,9 @@
       <c r="A51" s="1">
         <v>49</v>
       </c>
+      <c r="B51" s="7" t="s">
+        <v>409</v>
+      </c>
       <c r="C51" t="s">
         <v>269</v>
       </c>
@@ -15830,6 +16169,9 @@
       <c r="A52" s="1">
         <v>50</v>
       </c>
+      <c r="B52" s="7" t="s">
+        <v>410</v>
+      </c>
       <c r="C52" t="s">
         <v>269</v>
       </c>
@@ -15874,6 +16216,9 @@
       <c r="A53" s="1">
         <v>51</v>
       </c>
+      <c r="B53" s="7" t="s">
+        <v>411</v>
+      </c>
       <c r="C53" t="s">
         <v>269</v>
       </c>
@@ -15918,6 +16263,9 @@
       <c r="A54" s="1">
         <v>52</v>
       </c>
+      <c r="B54" s="7" t="s">
+        <v>412</v>
+      </c>
       <c r="C54" t="s">
         <v>269</v>
       </c>
@@ -15962,6 +16310,9 @@
       <c r="A55" s="1">
         <v>53</v>
       </c>
+      <c r="B55" t="s">
+        <v>413</v>
+      </c>
       <c r="C55" t="s">
         <v>269</v>
       </c>
@@ -16006,6 +16357,9 @@
       <c r="A56" s="1">
         <v>54</v>
       </c>
+      <c r="B56" t="s">
+        <v>414</v>
+      </c>
       <c r="C56" t="s">
         <v>269</v>
       </c>
@@ -16050,6 +16404,9 @@
       <c r="A57" s="1">
         <v>55</v>
       </c>
+      <c r="B57" t="s">
+        <v>415</v>
+      </c>
       <c r="C57" t="s">
         <v>269</v>
       </c>
@@ -16094,6 +16451,9 @@
       <c r="A58" s="1">
         <v>56</v>
       </c>
+      <c r="B58" t="s">
+        <v>416</v>
+      </c>
       <c r="C58" t="s">
         <v>269</v>
       </c>
@@ -16138,6 +16498,9 @@
       <c r="A59" s="1">
         <v>57</v>
       </c>
+      <c r="B59" t="s">
+        <v>417</v>
+      </c>
       <c r="C59" t="s">
         <v>269</v>
       </c>
@@ -16182,6 +16545,9 @@
       <c r="A60" s="1">
         <v>58</v>
       </c>
+      <c r="B60" t="s">
+        <v>418</v>
+      </c>
       <c r="C60" t="s">
         <v>269</v>
       </c>
@@ -16225,6 +16591,9 @@
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>419</v>
       </c>
       <c r="C61" t="s">
         <v>269</v>

</xml_diff>